<commit_message>
Results from July 20, 2020 10:57:27 PM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-20.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-20.xlsx
@@ -2438,25 +2438,25 @@
         </is>
       </c>
       <c r="B41" s="2" t="n">
-        <v>44032</v>
+        <v>44033</v>
       </c>
       <c r="C41" t="n">
-        <v>39251</v>
+        <v>39378</v>
       </c>
       <c r="D41" t="n">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="E41" t="n">
-        <v>3233</v>
+        <v>3238</v>
       </c>
       <c r="F41" t="n">
         <v>38</v>
       </c>
       <c r="G41" t="n">
-        <v>8.24</v>
+        <v>8.220000000000001</v>
       </c>
       <c r="H41" t="n">
-        <v>4.77</v>
+        <v>4.76</v>
       </c>
       <c r="I41" t="b">
         <v>1</v>

</xml_diff>